<commit_message>
Add Create BTO Exercise and Project
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ManagerList.xlsx
+++ b/src/main/resources/data/ManagerList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/hu0037ng_e_ntu_edu_sg/Documents/SC4079 - Final Year Project/SC2002/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2179e81e572d34a2/Documents/GitHub/sc2002_hdb_fcsd_group2/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC1048D321184AB85ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AED78119-22A7-4087-8472-22F30669F0DB}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC1048D321184AB85ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49A90C3E-2008-4CAD-A565-40390C5C0DC5}"/>
   <bookViews>
-    <workbookView xWindow="4057" yWindow="5932" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33090" yWindow="1155" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>TestUser</t>
   </si>
 </sst>
 </file>
@@ -113,6 +116,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,15 +385,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -420,7 +430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -435,6 +445,23 @@
       </c>
       <c r="E3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>